<commit_message>
CPT-280 feat: sort the excel by the lang key
</commit_message>
<xml_diff>
--- a/packages/i18n/excels/page-community.xlsx
+++ b/packages/i18n/excels/page-community.xlsx
@@ -22,187 +22,484 @@
     <t>en</t>
   </si>
   <si>
+    <t>/activities/activities/0/desc</t>
+  </si>
+  <si>
+    <t>TiDB Incubator Program is designed to ensure that new projects in the TiDB ecosystem can obtain resources and help from the community towards their desired maturity level.</t>
+  </si>
+  <si>
+    <t>/activities/activities/0/img</t>
+  </si>
+  <si>
+    <t>https://contributor.tidb.io/static/event-TiDB-Incubator-Program-1ade37389dac75fc23b1d408b2011973.svg</t>
+  </si>
+  <si>
+    <t>/activities/activities/0/link</t>
+  </si>
+  <si>
+    <t>https://github.com/pingcap/community/tree/master/incubator</t>
+  </si>
+  <si>
+    <t>/activities/activities/0/title</t>
+  </si>
+  <si>
+    <t>TiDB Incubator Program</t>
+  </si>
+  <si>
+    <t>/activities/activities/1/desc</t>
+  </si>
+  <si>
+    <t>The theme of Hackathon this year is [∞], by which we expect participants to innovate, to challenge, and to unlock the infinite power of TiDB.</t>
+  </si>
+  <si>
+    <t>/activities/activities/1/img</t>
+  </si>
+  <si>
+    <t>https://pingcap.com/static/tidb-hackathon2020-62c1c40e7dd9eb4a0eed8d00ea6507e5.jpg</t>
+  </si>
+  <si>
+    <t>/activities/activities/1/link</t>
+  </si>
+  <si>
+    <t>https://pingcap.com/community/events/hackathon2020/</t>
+  </si>
+  <si>
+    <t>/activities/activities/1/title</t>
+  </si>
+  <si>
+    <t>TiDB Hackathon 2020</t>
+  </si>
+  <si>
+    <t>/activities/activities/2/desc</t>
+  </si>
+  <si>
+    <t>High Performance TiDB Challenge is a mentoring program which focuses on workload optimization to bring TiDB performance to a higher level!</t>
+  </si>
+  <si>
+    <t>/activities/activities/2/img</t>
+  </si>
+  <si>
+    <t>https://pingcap.com/static/high-performance-tidb-challenge-ff7cb0ab67af3592ef7f1fe66151630c.png</t>
+  </si>
+  <si>
+    <t>/activities/activities/2/link</t>
+  </si>
+  <si>
+    <t>https://pingcap.com/community/events/high-performance-tidb-challenge/</t>
+  </si>
+  <si>
+    <t>/activities/activities/2/title</t>
+  </si>
+  <si>
+    <t>High Performance TiDB Challenge</t>
+  </si>
+  <si>
+    <t>/activities/desc</t>
+  </si>
+  <si>
+    <t>Meet other TiDB Community members IRL and online. Meet like-minded friends, share practical cases and technical experience.</t>
+  </si>
+  <si>
+    <t>/activities/title</t>
+  </si>
+  <si>
+    <t>Meet the TiDB Community</t>
+  </si>
+  <si>
+    <t>/activities/viewAll/label</t>
+  </si>
+  <si>
+    <t>View All Events</t>
+  </si>
+  <si>
+    <t>/activities/viewAll/link</t>
+  </si>
+  <si>
+    <t>https://contributor.tidb.io/events</t>
+  </si>
+  <si>
+    <t>/banner/desc</t>
+  </si>
+  <si>
+    <t>Join our community to learn, contribute, grow, and connect with TiDB contributors and users all around the world!</t>
+  </si>
+  <si>
+    <t>/banner/navs/0/isCN</t>
+  </si>
+  <si>
+    <t>/banner/navs/0/label</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>/banner/navs/0/link</t>
+  </si>
+  <si>
+    <t>https://asktug.com</t>
+  </si>
+  <si>
+    <t>/banner/navs/0/title</t>
+  </si>
+  <si>
+    <t>Forum</t>
+  </si>
+  <si>
+    <t>/banner/navs/1/label</t>
+  </si>
+  <si>
+    <t>Join</t>
+  </si>
+  <si>
+    <t>/banner/navs/1/link</t>
+  </si>
+  <si>
+    <t>https://slack.tidb.io/invite?team=tidb-community&amp;channel=everyone</t>
+  </si>
+  <si>
+    <t>/banner/navs/1/title</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>/banner/navs/2/label</t>
+  </si>
+  <si>
+    <t>Subscribe</t>
+  </si>
+  <si>
+    <t>/banner/navs/2/link</t>
+  </si>
+  <si>
+    <t>https://lists.tidb.io/g/main/subgroups</t>
+  </si>
+  <si>
+    <t>/banner/navs/2/title</t>
+  </si>
+  <si>
+    <t>Mailing List</t>
+  </si>
+  <si>
+    <t>/banner/navs/3/label</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>/banner/navs/3/link</t>
+  </si>
+  <si>
+    <t>https://docs.pingcap.com/tidb/stable</t>
+  </si>
+  <si>
+    <t>/banner/navs/3/title</t>
+  </si>
+  <si>
+    <t>Docs</t>
+  </si>
+  <si>
     <t>/banner/title</t>
   </si>
   <si>
     <t>Let’s build the database of the future together!</t>
   </si>
   <si>
-    <t>/banner/desc</t>
-  </si>
-  <si>
-    <t>Join our community to learn, contribute, grow, and connect with TiDB contributors and users all around the world!</t>
-  </si>
-  <si>
-    <t>/banner/navs/0/title</t>
-  </si>
-  <si>
-    <t>Forum</t>
-  </si>
-  <si>
-    <t>/banner/navs/0/label</t>
-  </si>
-  <si>
-    <t>View</t>
-  </si>
-  <si>
-    <t>/banner/navs/0/isCN</t>
-  </si>
-  <si>
-    <t>/banner/navs/0/link</t>
-  </si>
-  <si>
-    <t>https://asktug.com</t>
-  </si>
-  <si>
-    <t>/banner/navs/1/title</t>
-  </si>
-  <si>
-    <t>Slack</t>
-  </si>
-  <si>
-    <t>/banner/navs/1/label</t>
-  </si>
-  <si>
-    <t>Join</t>
-  </si>
-  <si>
-    <t>/banner/navs/1/link</t>
-  </si>
-  <si>
-    <t>https://slack.tidb.io/invite?team=tidb-community&amp;channel=everyone</t>
-  </si>
-  <si>
-    <t>/banner/navs/2/title</t>
-  </si>
-  <si>
-    <t>Mailing List</t>
-  </si>
-  <si>
-    <t>/banner/navs/2/label</t>
-  </si>
-  <si>
-    <t>Subscribe</t>
-  </si>
-  <si>
-    <t>/banner/navs/2/link</t>
-  </si>
-  <si>
-    <t>https://lists.tidb.io/g/main/subgroups</t>
-  </si>
-  <si>
-    <t>/banner/navs/3/title</t>
-  </si>
-  <si>
-    <t>Docs</t>
-  </si>
-  <si>
-    <t>/banner/navs/3/label</t>
-  </si>
-  <si>
-    <t>Read</t>
-  </si>
-  <si>
-    <t>/banner/navs/3/link</t>
-  </si>
-  <si>
-    <t>https://docs.pingcap.com/tidb/stable</t>
-  </si>
-  <si>
-    <t>/activities/title</t>
-  </si>
-  <si>
-    <t>Meet the TiDB Community</t>
-  </si>
-  <si>
-    <t>/activities/desc</t>
-  </si>
-  <si>
-    <t>Meet other TiDB Community members IRL and online. Meet like-minded friends, share practical cases and technical experience.</t>
-  </si>
-  <si>
-    <t>/activities/activities/0/title</t>
-  </si>
-  <si>
-    <t>TiDB Incubator Program</t>
-  </si>
-  <si>
-    <t>/activities/activities/0/desc</t>
-  </si>
-  <si>
-    <t>TiDB Incubator Program is designed to ensure that new projects in the TiDB ecosystem can obtain resources and help from the community towards their desired maturity level.</t>
-  </si>
-  <si>
-    <t>/activities/activities/0/link</t>
-  </si>
-  <si>
-    <t>https://github.com/pingcap/community/tree/master/incubator</t>
-  </si>
-  <si>
-    <t>/activities/activities/0/img</t>
-  </si>
-  <si>
-    <t>https://contributor.tidb.io/static/event-TiDB-Incubator-Program-1ade37389dac75fc23b1d408b2011973.svg</t>
-  </si>
-  <si>
-    <t>/activities/activities/1/title</t>
-  </si>
-  <si>
-    <t>TiDB Hackathon 2020</t>
-  </si>
-  <si>
-    <t>/activities/activities/1/desc</t>
-  </si>
-  <si>
-    <t>The theme of Hackathon this year is [∞], by which we expect participants to innovate, to challenge, and to unlock the infinite power of TiDB.</t>
-  </si>
-  <si>
-    <t>/activities/activities/1/link</t>
-  </si>
-  <si>
-    <t>https://pingcap.com/community/events/hackathon2020/</t>
-  </si>
-  <si>
-    <t>/activities/activities/1/img</t>
-  </si>
-  <si>
-    <t>https://pingcap.com/static/tidb-hackathon2020-62c1c40e7dd9eb4a0eed8d00ea6507e5.jpg</t>
-  </si>
-  <si>
-    <t>/activities/activities/2/title</t>
-  </si>
-  <si>
-    <t>High Performance TiDB Challenge</t>
-  </si>
-  <si>
-    <t>/activities/activities/2/desc</t>
-  </si>
-  <si>
-    <t>High Performance TiDB Challenge is a mentoring program which focuses on workload optimization to bring TiDB performance to a higher level!</t>
-  </si>
-  <si>
-    <t>/activities/activities/2/link</t>
-  </si>
-  <si>
-    <t>https://pingcap.com/community/events/high-performance-tidb-challenge/</t>
-  </si>
-  <si>
-    <t>/activities/activities/2/img</t>
-  </si>
-  <si>
-    <t>https://pingcap.com/static/high-performance-tidb-challenge-ff7cb0ab67af3592ef7f1fe66151630c.png</t>
-  </si>
-  <si>
-    <t>/activities/viewAll/label</t>
-  </si>
-  <si>
-    <t>View All Events</t>
-  </si>
-  <si>
-    <t>/activities/viewAll/link</t>
-  </si>
-  <si>
-    <t>https://contributor.tidb.io/events</t>
+    <t>/career/certTitle</t>
+  </si>
+  <si>
+    <t>Certification</t>
+  </si>
+  <si>
+    <t>/career/desc</t>
+  </si>
+  <si>
+    <t>Here you can find attractive job opportunities posted by TiDB users. It’s free to post and apply for a job. Wish you the best of luck in your search!</t>
+  </si>
+  <si>
+    <t>/career/job/items/0/iconId</t>
+  </si>
+  <si>
+    <t>paypay</t>
+  </si>
+  <si>
+    <t>/career/job/items/0/linkId</t>
+  </si>
+  <si>
+    <t>paypay/dba</t>
+  </si>
+  <si>
+    <t>/career/job/items/0/location</t>
+  </si>
+  <si>
+    <t>上海</t>
+  </si>
+  <si>
+    <t>/career/job/items/0/position</t>
+  </si>
+  <si>
+    <t>资深 DBA 工程师</t>
+  </si>
+  <si>
+    <t>/career/job/items/1/iconId</t>
+  </si>
+  <si>
+    <t>yichewang</t>
+  </si>
+  <si>
+    <t>/career/job/items/1/linkId</t>
+  </si>
+  <si>
+    <t>yichewang/dba</t>
+  </si>
+  <si>
+    <t>/career/job/items/1/location</t>
+  </si>
+  <si>
+    <t>北京</t>
+  </si>
+  <si>
+    <t>/career/job/items/1/position</t>
+  </si>
+  <si>
+    <t>DBA</t>
+  </si>
+  <si>
+    <t>/career/job/items/2/iconId</t>
+  </si>
+  <si>
+    <t>zhangmen</t>
+  </si>
+  <si>
+    <t>/career/job/items/2/linkId</t>
+  </si>
+  <si>
+    <t>zhangmen/dba-tidb</t>
+  </si>
+  <si>
+    <t>/career/job/items/2/location</t>
+  </si>
+  <si>
+    <t>/career/job/items/2/position</t>
+  </si>
+  <si>
+    <t>DBA - TiDB 专岗</t>
+  </si>
+  <si>
+    <t>/career/job/items/3/iconId</t>
+  </si>
+  <si>
+    <t>huya</t>
+  </si>
+  <si>
+    <t>/career/job/items/3/linkId</t>
+  </si>
+  <si>
+    <t>huya/dba</t>
+  </si>
+  <si>
+    <t>/career/job/items/3/location</t>
+  </si>
+  <si>
+    <t>广州</t>
+  </si>
+  <si>
+    <t>/career/job/items/3/position</t>
+  </si>
+  <si>
+    <t>DBA 工程师</t>
+  </si>
+  <si>
+    <t>/career/job/items/4/iconId</t>
+  </si>
+  <si>
+    <t>xiaomi</t>
+  </si>
+  <si>
+    <t>/career/job/items/4/linkId</t>
+  </si>
+  <si>
+    <t>xiaomi/dba</t>
+  </si>
+  <si>
+    <t>/career/job/items/4/location</t>
+  </si>
+  <si>
+    <t>/career/job/items/4/position</t>
+  </si>
+  <si>
+    <t>/career/job/items/5/iconId</t>
+  </si>
+  <si>
+    <t>kingSoft</t>
+  </si>
+  <si>
+    <t>/career/job/items/5/linkId</t>
+  </si>
+  <si>
+    <t>kingsoft/dba</t>
+  </si>
+  <si>
+    <t>/career/job/items/5/location</t>
+  </si>
+  <si>
+    <t>广州/珠海</t>
+  </si>
+  <si>
+    <t>/career/job/items/5/position</t>
+  </si>
+  <si>
+    <t>DBA 运维开发</t>
+  </si>
+  <si>
+    <t>/career/job/items/6/iconId</t>
+  </si>
+  <si>
+    <t>ucloud</t>
+  </si>
+  <si>
+    <t>/career/job/items/6/linkId</t>
+  </si>
+  <si>
+    <t>go-engineer-paas</t>
+  </si>
+  <si>
+    <t>/career/job/items/6/location</t>
+  </si>
+  <si>
+    <t>/career/job/items/6/position</t>
+  </si>
+  <si>
+    <t>Go 研发工程师</t>
+  </si>
+  <si>
+    <t>/career/job/items/7/iconId</t>
+  </si>
+  <si>
+    <t>/career/job/items/7/linkId</t>
+  </si>
+  <si>
+    <t>go-engineer-tidb</t>
+  </si>
+  <si>
+    <t>/career/job/items/7/location</t>
+  </si>
+  <si>
+    <t>/career/job/items/7/position</t>
+  </si>
+  <si>
+    <t>/career/job/title</t>
+  </si>
+  <si>
+    <t>Job Board</t>
+  </si>
+  <si>
+    <t>/career/job/viewAll/label</t>
+  </si>
+  <si>
+    <t>View More Opportunities</t>
+  </si>
+  <si>
+    <t>/career/job/viewAll/link</t>
+  </si>
+  <si>
+    <t>https://tidb-jobs.pingcap.com</t>
+  </si>
+  <si>
+    <t>/career/title</t>
+  </si>
+  <si>
+    <t>Career</t>
+  </si>
+  <si>
+    <t>/contributor/items/0/desc</t>
+  </si>
+  <si>
+    <t>Development workflow, commit message formatting, contact points and other resources.</t>
+  </si>
+  <si>
+    <t>/contributor/items/0/link</t>
+  </si>
+  <si>
+    <t>https://github.com/pingcap/community/blob/master/contributors/README.md</t>
+  </si>
+  <si>
+    <t>/contributor/items/0/title</t>
+  </si>
+  <si>
+    <t>Contributing Guide</t>
+  </si>
+  <si>
+    <t>/contributor/items/1/desc</t>
+  </si>
+  <si>
+    <t>Learning knowledge and skills, sharing best practices, become a database expert, develop database standards.</t>
+  </si>
+  <si>
+    <t>/contributor/items/1/link</t>
+  </si>
+  <si>
+    <t>https://contributor.tidb.io</t>
+  </si>
+  <si>
+    <t>/contributor/items/1/title</t>
+  </si>
+  <si>
+    <t>Join Developer Group</t>
+  </si>
+  <si>
+    <t>/contributor/items/2/desc</t>
+  </si>
+  <si>
+    <t>Agreement on rules of behaviour for the members of TiDB Community.</t>
+  </si>
+  <si>
+    <t>/contributor/items/2/link</t>
+  </si>
+  <si>
+    <t>https://github.com/pingcap/community/blob/master/CODE_OF_CONDUCT.md</t>
+  </si>
+  <si>
+    <t>/contributor/items/2/title</t>
+  </si>
+  <si>
+    <t>Code of Conduct</t>
+  </si>
+  <si>
+    <t>/contributor/title</t>
+  </si>
+  <si>
+    <t>Become a Contributor</t>
+  </si>
+  <si>
+    <t>/learning/btns/docs/label</t>
+  </si>
+  <si>
+    <t>/learning/btns/docs/link</t>
+  </si>
+  <si>
+    <t>/learning/btns/pu/label</t>
+  </si>
+  <si>
+    <t>PingCAP University</t>
+  </si>
+  <si>
+    <t>/learning/btns/pu/link</t>
+  </si>
+  <si>
+    <t>https://university.pingcap.com</t>
+  </si>
+  <si>
+    <t>/learning/desc/0</t>
+  </si>
+  <si>
+    <t>PingCAP University is committed to cultivating first-class talents in developing, managing and applying distributed relational database systems. All training and certification courses are designed and taught by the official TiDB technical experts of PingCAP.</t>
+  </si>
+  <si>
+    <t>/learning/desc/1</t>
+  </si>
+  <si>
+    <t>You can also read the official document to learn the usage of TiDB.</t>
   </si>
   <si>
     <t>/learning/title</t>
@@ -211,331 +508,34 @@
     <t>Learn How to Use TiDB</t>
   </si>
   <si>
-    <t>/learning/desc/0</t>
-  </si>
-  <si>
-    <t>PingCAP University is committed to cultivating first-class talents in developing, managing and applying distributed relational database systems. All training and certification courses are designed and taught by the official TiDB technical experts of PingCAP.</t>
-  </si>
-  <si>
-    <t>/learning/desc/1</t>
-  </si>
-  <si>
-    <t>You can also read the official document to learn the usage of TiDB.</t>
-  </si>
-  <si>
-    <t>/learning/btns/pu/label</t>
-  </si>
-  <si>
-    <t>PingCAP University</t>
-  </si>
-  <si>
-    <t>/learning/btns/pu/link</t>
-  </si>
-  <si>
-    <t>https://university.pingcap.com</t>
-  </si>
-  <si>
-    <t>/learning/btns/docs/label</t>
-  </si>
-  <si>
-    <t>/learning/btns/docs/link</t>
+    <t>/userGroup/btns/ask/label</t>
+  </si>
+  <si>
+    <t>/userGroup/btns/ask/link</t>
+  </si>
+  <si>
+    <t>/userGroup/btns/join/label</t>
+  </si>
+  <si>
+    <t>Join TUG</t>
+  </si>
+  <si>
+    <t>/userGroup/btns/join/link</t>
+  </si>
+  <si>
+    <t>https://tug.tidb.io</t>
+  </si>
+  <si>
+    <t>/userGroup/desc</t>
+  </si>
+  <si>
+    <t>TUG (TiDB User Group) is an independent, self-organized, and non-profit organization that gathers the database and big data technology practitioners around the world. In TUG, you can increase your personal influence, open up your horizons and make like-minded friends.</t>
   </si>
   <si>
     <t>/userGroup/title</t>
   </si>
   <si>
     <t>Join User Group</t>
-  </si>
-  <si>
-    <t>/userGroup/desc</t>
-  </si>
-  <si>
-    <t>TUG (TiDB User Group) is an independent, self-organized, and non-profit organization that gathers the database and big data technology practitioners around the world. In TUG, you can increase your personal influence, open up your horizons and make like-minded friends.</t>
-  </si>
-  <si>
-    <t>/userGroup/btns/join/label</t>
-  </si>
-  <si>
-    <t>Join TUG</t>
-  </si>
-  <si>
-    <t>/userGroup/btns/join/link</t>
-  </si>
-  <si>
-    <t>https://tug.tidb.io</t>
-  </si>
-  <si>
-    <t>/userGroup/btns/ask/label</t>
-  </si>
-  <si>
-    <t>/userGroup/btns/ask/link</t>
-  </si>
-  <si>
-    <t>/contributor/title</t>
-  </si>
-  <si>
-    <t>Become a Contributor</t>
-  </si>
-  <si>
-    <t>/contributor/items/0/title</t>
-  </si>
-  <si>
-    <t>Contributing Guide</t>
-  </si>
-  <si>
-    <t>/contributor/items/0/desc</t>
-  </si>
-  <si>
-    <t>Development workflow, commit message formatting, contact points and other resources.</t>
-  </si>
-  <si>
-    <t>/contributor/items/0/link</t>
-  </si>
-  <si>
-    <t>https://github.com/pingcap/community/blob/master/contributors/README.md</t>
-  </si>
-  <si>
-    <t>/contributor/items/1/title</t>
-  </si>
-  <si>
-    <t>Join Developer Group</t>
-  </si>
-  <si>
-    <t>/contributor/items/1/desc</t>
-  </si>
-  <si>
-    <t>Learning knowledge and skills, sharing best practices, become a database expert, develop database standards.</t>
-  </si>
-  <si>
-    <t>/contributor/items/1/link</t>
-  </si>
-  <si>
-    <t>https://contributor.tidb.io</t>
-  </si>
-  <si>
-    <t>/contributor/items/2/title</t>
-  </si>
-  <si>
-    <t>Code of Conduct</t>
-  </si>
-  <si>
-    <t>/contributor/items/2/desc</t>
-  </si>
-  <si>
-    <t>Agreement on rules of behaviour for the members of TiDB Community.</t>
-  </si>
-  <si>
-    <t>/contributor/items/2/link</t>
-  </si>
-  <si>
-    <t>https://github.com/pingcap/community/blob/master/CODE_OF_CONDUCT.md</t>
-  </si>
-  <si>
-    <t>/career/title</t>
-  </si>
-  <si>
-    <t>Career</t>
-  </si>
-  <si>
-    <t>/career/desc</t>
-  </si>
-  <si>
-    <t>Here you can find attractive job opportunities posted by TiDB users. It’s free to post and apply for a job. Wish you the best of luck in your search!</t>
-  </si>
-  <si>
-    <t>/career/certTitle</t>
-  </si>
-  <si>
-    <t>Certification</t>
-  </si>
-  <si>
-    <t>/career/job/title</t>
-  </si>
-  <si>
-    <t>Job Board</t>
-  </si>
-  <si>
-    <t>/career/job/viewAll/label</t>
-  </si>
-  <si>
-    <t>View More Opportunities</t>
-  </si>
-  <si>
-    <t>/career/job/viewAll/link</t>
-  </si>
-  <si>
-    <t>https://tidb-jobs.pingcap.com</t>
-  </si>
-  <si>
-    <t>/career/job/items/0/iconId</t>
-  </si>
-  <si>
-    <t>paypay</t>
-  </si>
-  <si>
-    <t>/career/job/items/0/position</t>
-  </si>
-  <si>
-    <t>资深 DBA 工程师</t>
-  </si>
-  <si>
-    <t>/career/job/items/0/location</t>
-  </si>
-  <si>
-    <t>上海</t>
-  </si>
-  <si>
-    <t>/career/job/items/0/linkId</t>
-  </si>
-  <si>
-    <t>paypay/dba</t>
-  </si>
-  <si>
-    <t>/career/job/items/1/iconId</t>
-  </si>
-  <si>
-    <t>yichewang</t>
-  </si>
-  <si>
-    <t>/career/job/items/1/position</t>
-  </si>
-  <si>
-    <t>DBA</t>
-  </si>
-  <si>
-    <t>/career/job/items/1/location</t>
-  </si>
-  <si>
-    <t>北京</t>
-  </si>
-  <si>
-    <t>/career/job/items/1/linkId</t>
-  </si>
-  <si>
-    <t>yichewang/dba</t>
-  </si>
-  <si>
-    <t>/career/job/items/2/iconId</t>
-  </si>
-  <si>
-    <t>zhangmen</t>
-  </si>
-  <si>
-    <t>/career/job/items/2/position</t>
-  </si>
-  <si>
-    <t>DBA - TiDB 专岗</t>
-  </si>
-  <si>
-    <t>/career/job/items/2/location</t>
-  </si>
-  <si>
-    <t>/career/job/items/2/linkId</t>
-  </si>
-  <si>
-    <t>zhangmen/dba-tidb</t>
-  </si>
-  <si>
-    <t>/career/job/items/3/iconId</t>
-  </si>
-  <si>
-    <t>huya</t>
-  </si>
-  <si>
-    <t>/career/job/items/3/position</t>
-  </si>
-  <si>
-    <t>DBA 工程师</t>
-  </si>
-  <si>
-    <t>/career/job/items/3/location</t>
-  </si>
-  <si>
-    <t>广州</t>
-  </si>
-  <si>
-    <t>/career/job/items/3/linkId</t>
-  </si>
-  <si>
-    <t>huya/dba</t>
-  </si>
-  <si>
-    <t>/career/job/items/4/iconId</t>
-  </si>
-  <si>
-    <t>xiaomi</t>
-  </si>
-  <si>
-    <t>/career/job/items/4/position</t>
-  </si>
-  <si>
-    <t>/career/job/items/4/location</t>
-  </si>
-  <si>
-    <t>/career/job/items/4/linkId</t>
-  </si>
-  <si>
-    <t>xiaomi/dba</t>
-  </si>
-  <si>
-    <t>/career/job/items/5/iconId</t>
-  </si>
-  <si>
-    <t>kingSoft</t>
-  </si>
-  <si>
-    <t>/career/job/items/5/position</t>
-  </si>
-  <si>
-    <t>DBA 运维开发</t>
-  </si>
-  <si>
-    <t>/career/job/items/5/location</t>
-  </si>
-  <si>
-    <t>广州/珠海</t>
-  </si>
-  <si>
-    <t>/career/job/items/5/linkId</t>
-  </si>
-  <si>
-    <t>kingsoft/dba</t>
-  </si>
-  <si>
-    <t>/career/job/items/6/iconId</t>
-  </si>
-  <si>
-    <t>ucloud</t>
-  </si>
-  <si>
-    <t>/career/job/items/6/position</t>
-  </si>
-  <si>
-    <t>Go 研发工程师</t>
-  </si>
-  <si>
-    <t>/career/job/items/6/location</t>
-  </si>
-  <si>
-    <t>/career/job/items/6/linkId</t>
-  </si>
-  <si>
-    <t>go-engineer-paas</t>
-  </si>
-  <si>
-    <t>/career/job/items/7/iconId</t>
-  </si>
-  <si>
-    <t>/career/job/items/7/position</t>
-  </si>
-  <si>
-    <t>/career/job/items/7/location</t>
-  </si>
-  <si>
-    <t>/career/job/items/7/linkId</t>
-  </si>
-  <si>
-    <t>go-engineer-tidb</t>
   </si>
 </sst>
 </file>
@@ -1006,125 +1006,125 @@
         <v>11</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5" t="b">
-        <v>1</v>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
+      <c r="C19" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1295,214 +1295,214 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1520,160 +1520,160 @@
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1682,106 +1682,106 @@
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5" t="s">
-        <v>154</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5" t="s">
-        <v>156</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5" t="s">
-        <v>123</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5" t="s">
-        <v>169</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>